<commit_message>
chore: update simulation name
modified:   ../TDD_examples/CASE_2_ENEA_HTS_CICC/transitory_input.xlsx
modified:   ../TDD_examples/CASE_3_HTS_HVDC/transitory_input.xlsx
</commit_message>
<xml_diff>
--- a/TDD_examples/CASE_2_ENEA_HTS_CICC/transitory_input.xlsx
+++ b/TDD_examples/CASE_2_ENEA_HTS_CICC/transitory_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/SC2/Description_of_Components/Cavo_ENEA_input_whole/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\TDD_examples\CASE_2_ENEA_HTS_CICC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{6E8367A2-355C-4B5A-B49E-C4946B093F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55CE8A5E-6145-4C2B-B608-FF39EAD53B54}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE5EEFC-625C-4DAE-875D-723A62F0A540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRANSIENT" sheetId="1" r:id="rId1"/>
@@ -186,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -207,19 +207,11 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,24 +558,24 @@
       <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="95.81640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="3"/>
+    <col min="6" max="6" width="95.85546875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -600,7 +592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -613,12 +605,12 @@
       <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="8" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,A6,E6,A8,E8,[1]GRID!$A$4,[1]GRID!$E$4,"refined")</f>
-        <v>TEND_50_STPMIN_0.05_NELEMS_150_refined</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,A6,E6,A8,E8,[1]GRID!$A$4,[1]GRID!$E$4,"case2")</f>
+        <v>TEND_50_STPMIN_0.05_NELEMS_150_case2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -631,28 +623,28 @@
       <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -665,11 +657,11 @@
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -682,11 +674,11 @@
       <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -699,11 +691,11 @@
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -720,7 +712,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -733,11 +725,11 @@
       <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -750,7 +742,7 @@
       <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="2">
         <v>5</v>
       </c>
     </row>

</xml_diff>